<commit_message>
Added unit test for FX option in xVALite.
</commit_message>
<xml_diff>
--- a/tests/fx-option-atm-vol-surface.xlsx
+++ b/tests/fx-option-atm-vol-surface.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nerasmus\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitLab\stochastic_process_calibration_2022\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46BFC3A-9A3D-4C09-B3BE-8331B9E7626E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0547CB86-2F05-4111-92A1-913496BDE2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28690" yWindow="-110" windowWidth="29020" windowHeight="15820" xr2:uid="{E45817EA-4355-45A7-9B27-4C7906A9F58A}"/>
+    <workbookView xWindow="-19140" yWindow="2040" windowWidth="15360" windowHeight="8100" xr2:uid="{E45817EA-4355-45A7-9B27-4C7906A9F58A}"/>
   </bookViews>
   <sheets>
     <sheet name="vol_surface" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +46,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,12 +67,6 @@
     <font>
       <sz val="9"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,7 +96,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -122,26 +120,62 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="1"/>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
-      <right/>
-      <top style="hair">
-        <color theme="1"/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="1"/>
+        <color indexed="64"/>
       </left>
-      <right/>
-      <top style="hair">
-        <color theme="1"/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color theme="1"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -149,19 +183,15 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Borders" xfId="1" xr:uid="{B2521F41-D53A-4512-B4C5-E85D0D4D431D}"/>
@@ -481,12 +511,12 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,131 +524,131 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0.02</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="3">
         <v>13.25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>0.08</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>0.17</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>14.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>0.25</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>14.85</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>0.5</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>15.4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>0.75</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>15.55</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>15.55</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>15.75</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>3</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>16.149999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>4</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>16.350000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>5</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>16.850000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>6</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>17.350000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>7</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>17.850000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>8</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>18.45</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>9</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>19.05</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="3">
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
         <v>10</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="5">
         <v>19.649999999999999</v>
       </c>
     </row>

</xml_diff>